<commit_message>
fixed a codes in S13.csv controlled vocabulary
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-organizations/S13/S13.xlsx
+++ b/VocabolariControllati/classifications-for-organizations/S13/S13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-organizations/S13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449700DB-1A01-B249-A684-4227CD9E7E0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217D0E2-2A45-C047-8BC4-A00C0DBEA563}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="460" windowWidth="23680" windowHeight="13560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,13 +723,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="357">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1427,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="169" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,13 +1463,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1479,13 +1480,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1496,13 +1497,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>108</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1513,13 +1514,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>103</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1530,13 +1531,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>104</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1547,13 +1548,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>105</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1564,13 +1565,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1581,13 +1582,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1598,13 +1599,13 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>107</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1615,13 +1616,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>110</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1632,13 +1633,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>112</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1649,13 +1650,13 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>201</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1666,13 +1667,13 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>203</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1683,13 +1684,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>202</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1700,13 +1701,13 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>204</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1717,13 +1718,13 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>205</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1734,13 +1735,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>206</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1751,13 +1752,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="3">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>216</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1768,13 +1769,13 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>212</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1788,13 +1789,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="3">
         <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>222</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1808,13 +1809,13 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="3">
         <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>220</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1825,13 +1826,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="3">
         <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>233</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1845,13 +1846,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="3">
         <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>232</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1862,13 +1863,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="3">
         <v>2</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>221</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1879,13 +1880,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="3">
         <v>2</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>225</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1896,13 +1897,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="3">
         <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>218</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1913,13 +1914,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="3">
         <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>208</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1933,13 +1934,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="3">
         <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>207</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1950,13 +1951,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="3">
         <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>211</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1967,13 +1968,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="3">
         <v>2</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>224</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1984,13 +1985,13 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="3">
         <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>237</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2001,13 +2002,13 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="3">
         <v>2</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>219</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -2021,13 +2022,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="3">
         <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>230</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2038,13 +2039,13 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="3">
         <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="3">
         <v>217</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2058,13 +2059,13 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="3">
         <v>2</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>239</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -2075,13 +2076,13 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>2</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>234</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -2092,13 +2093,13 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="3">
         <v>2</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>213</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2112,13 +2113,13 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="3">
         <v>2</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>223</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2132,13 +2133,13 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="3">
         <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>300</v>
       </c>
       <c r="D40" s="1" t="s">

</xml_diff>